<commit_message>
experimental results for mean, mode, and stdev aggregation formulas
</commit_message>
<xml_diff>
--- a/experiment_results/20201127_AGGREGATION_MEDIAN_NORMALIZATION1/BankAccountTP/4wise/0.95_.xlsx
+++ b/experiment_results/20201127_AGGREGATION_MEDIAN_NORMALIZATION1/BankAccountTP/4wise/0.95_.xlsx
@@ -788,19 +788,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -864,19 +864,19 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <v>38</v>
       </c>
       <c r="E11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G11">
         <v>76</v>
@@ -940,7 +940,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -949,7 +949,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -1016,7 +1016,7 @@
         <v>25</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -1025,7 +1025,7 @@
         <v>34</v>
       </c>
       <c r="E15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F15">
         <v>3</v>
@@ -1063,10 +1063,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -1104,7 +1104,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -1168,19 +1168,19 @@
         <v>29</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>36</v>
       </c>
       <c r="E19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G19">
         <v>76</v>
@@ -1282,16 +1282,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -1637,19 +1637,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -1789,7 +1789,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1798,7 +1798,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -1912,10 +1912,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -1953,7 +1953,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -2131,16 +2131,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -2486,19 +2486,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -2638,7 +2638,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -2647,7 +2647,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -2761,10 +2761,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -2802,7 +2802,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -2980,16 +2980,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -3335,19 +3335,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -3487,7 +3487,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -3496,7 +3496,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -3610,10 +3610,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -3651,7 +3651,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -3715,10 +3715,10 @@
         <v>29</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>36</v>
@@ -3829,16 +3829,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -4184,19 +4184,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -4336,7 +4336,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -4345,7 +4345,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -4459,10 +4459,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -4500,7 +4500,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -4564,10 +4564,10 @@
         <v>29</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>36</v>
@@ -4678,16 +4678,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -5033,19 +5033,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -5185,7 +5185,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -5194,7 +5194,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -5308,10 +5308,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -5349,7 +5349,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -5527,16 +5527,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -5882,19 +5882,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -6034,7 +6034,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -6043,7 +6043,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -6157,10 +6157,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -6198,7 +6198,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -6376,16 +6376,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -7006,7 +7006,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F16">
         <v>10</v>
@@ -7234,7 +7234,7 @@
         <v>20</v>
       </c>
       <c r="E22">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F22">
         <v>12</v>
@@ -7352,19 +7352,19 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>23</v>
       </c>
       <c r="E3">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F3">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>76</v>
@@ -7399,10 +7399,10 @@
         <v>17</v>
       </c>
       <c r="E4">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <v>76</v>
@@ -7437,10 +7437,10 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F5">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G5">
         <v>76</v>
@@ -7475,10 +7475,10 @@
         <v>11</v>
       </c>
       <c r="E6">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F6">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G6">
         <v>76</v>
@@ -7513,10 +7513,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G7">
         <v>76</v>
@@ -7542,19 +7542,19 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G8">
         <v>76</v>
@@ -7580,10 +7580,10 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
@@ -7627,10 +7627,10 @@
         <v>16</v>
       </c>
       <c r="E10">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="F10">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="G10">
         <v>76</v>
@@ -7732,7 +7732,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -7741,10 +7741,10 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="G13">
         <v>76</v>
@@ -7779,10 +7779,10 @@
         <v>24</v>
       </c>
       <c r="E14">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F14">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G14">
         <v>76</v>
@@ -7808,19 +7808,19 @@
         <v>25</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15">
         <v>34</v>
       </c>
       <c r="E15">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F15">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G15">
         <v>76</v>
@@ -7855,10 +7855,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F16">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -7893,10 +7893,10 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F17">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -7931,10 +7931,10 @@
         <v>11</v>
       </c>
       <c r="E18">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G18">
         <v>76</v>
@@ -7960,19 +7960,19 @@
         <v>29</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D19">
         <v>36</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G19">
         <v>76</v>
@@ -8045,10 +8045,10 @@
         <v>21</v>
       </c>
       <c r="E21">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="F21">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G21">
         <v>76</v>
@@ -8074,10 +8074,10 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
@@ -8086,7 +8086,7 @@
         <v>41</v>
       </c>
       <c r="F22">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G22">
         <v>76</v>
@@ -8429,19 +8429,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -8581,7 +8581,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -8590,7 +8590,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -8704,10 +8704,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -8745,7 +8745,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -8923,16 +8923,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -9278,19 +9278,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -9430,7 +9430,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -9439,7 +9439,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -9553,10 +9553,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -9594,7 +9594,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -9772,16 +9772,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -10127,19 +10127,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -10279,7 +10279,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -10288,7 +10288,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -10402,10 +10402,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -10443,7 +10443,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -10621,16 +10621,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -10748,19 +10748,19 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>23</v>
       </c>
       <c r="E3">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F3">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>76</v>
@@ -10795,10 +10795,10 @@
         <v>17</v>
       </c>
       <c r="E4">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <v>76</v>
@@ -10833,10 +10833,10 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F5">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G5">
         <v>76</v>
@@ -10871,10 +10871,10 @@
         <v>11</v>
       </c>
       <c r="E6">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F6">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G6">
         <v>76</v>
@@ -10909,10 +10909,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G7">
         <v>76</v>
@@ -10938,19 +10938,19 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G8">
         <v>76</v>
@@ -10976,10 +10976,10 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
@@ -11023,10 +11023,10 @@
         <v>16</v>
       </c>
       <c r="E10">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="F10">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="G10">
         <v>76</v>
@@ -11128,7 +11128,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -11137,10 +11137,10 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="G13">
         <v>76</v>
@@ -11175,10 +11175,10 @@
         <v>24</v>
       </c>
       <c r="E14">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F14">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G14">
         <v>76</v>
@@ -11204,19 +11204,19 @@
         <v>25</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15">
         <v>34</v>
       </c>
       <c r="E15">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F15">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G15">
         <v>76</v>
@@ -11251,10 +11251,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F16">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -11289,10 +11289,10 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F17">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -11327,10 +11327,10 @@
         <v>11</v>
       </c>
       <c r="E18">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G18">
         <v>76</v>
@@ -11356,19 +11356,19 @@
         <v>29</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D19">
         <v>36</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G19">
         <v>76</v>
@@ -11441,10 +11441,10 @@
         <v>21</v>
       </c>
       <c r="E21">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="F21">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G21">
         <v>76</v>
@@ -11470,10 +11470,10 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
@@ -11482,7 +11482,7 @@
         <v>41</v>
       </c>
       <c r="F22">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G22">
         <v>76</v>
@@ -11597,19 +11597,19 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>23</v>
       </c>
       <c r="E3">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F3">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>76</v>
@@ -11644,10 +11644,10 @@
         <v>17</v>
       </c>
       <c r="E4">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <v>76</v>
@@ -11682,10 +11682,10 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F5">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G5">
         <v>76</v>
@@ -11720,10 +11720,10 @@
         <v>11</v>
       </c>
       <c r="E6">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F6">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G6">
         <v>76</v>
@@ -11758,10 +11758,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G7">
         <v>76</v>
@@ -11787,19 +11787,19 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G8">
         <v>76</v>
@@ -11825,10 +11825,10 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
@@ -11872,10 +11872,10 @@
         <v>16</v>
       </c>
       <c r="E10">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="F10">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="G10">
         <v>76</v>
@@ -11977,7 +11977,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -11986,10 +11986,10 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="G13">
         <v>76</v>
@@ -12024,10 +12024,10 @@
         <v>24</v>
       </c>
       <c r="E14">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F14">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G14">
         <v>76</v>
@@ -12053,19 +12053,19 @@
         <v>25</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15">
         <v>34</v>
       </c>
       <c r="E15">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F15">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G15">
         <v>76</v>
@@ -12100,10 +12100,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F16">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -12138,10 +12138,10 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F17">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -12176,10 +12176,10 @@
         <v>11</v>
       </c>
       <c r="E18">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G18">
         <v>76</v>
@@ -12205,19 +12205,19 @@
         <v>29</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D19">
         <v>36</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G19">
         <v>76</v>
@@ -12290,10 +12290,10 @@
         <v>21</v>
       </c>
       <c r="E21">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="F21">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G21">
         <v>76</v>
@@ -12319,10 +12319,10 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
@@ -12331,7 +12331,7 @@
         <v>41</v>
       </c>
       <c r="F22">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G22">
         <v>76</v>
@@ -12446,19 +12446,19 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>23</v>
       </c>
       <c r="E3">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F3">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G3">
         <v>76</v>
@@ -12493,10 +12493,10 @@
         <v>17</v>
       </c>
       <c r="E4">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <v>76</v>
@@ -12531,10 +12531,10 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F5">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G5">
         <v>76</v>
@@ -12569,10 +12569,10 @@
         <v>11</v>
       </c>
       <c r="E6">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G6">
         <v>76</v>
@@ -12607,10 +12607,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G7">
         <v>76</v>
@@ -12636,19 +12636,19 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G8">
         <v>76</v>
@@ -12674,19 +12674,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F9">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -12721,10 +12721,10 @@
         <v>16</v>
       </c>
       <c r="E10">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F10">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G10">
         <v>76</v>
@@ -12826,19 +12826,19 @@
         <v>23</v>
       </c>
       <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>23</v>
+      </c>
+      <c r="E13">
         <v>6</v>
       </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>23</v>
-      </c>
-      <c r="E13">
-        <v>17</v>
-      </c>
       <c r="F13">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="G13">
         <v>76</v>
@@ -12873,10 +12873,10 @@
         <v>24</v>
       </c>
       <c r="E14">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F14">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="G14">
         <v>76</v>
@@ -12911,10 +12911,10 @@
         <v>34</v>
       </c>
       <c r="E15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G15">
         <v>76</v>
@@ -12949,10 +12949,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F16">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -12987,10 +12987,10 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F17">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -13025,10 +13025,10 @@
         <v>11</v>
       </c>
       <c r="E18">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G18">
         <v>76</v>
@@ -13054,10 +13054,10 @@
         <v>29</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>36</v>
@@ -13139,10 +13139,10 @@
         <v>21</v>
       </c>
       <c r="E21">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F21">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G21">
         <v>76</v>
@@ -13168,19 +13168,19 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G22">
         <v>76</v>
@@ -13523,19 +13523,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -13675,7 +13675,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -13684,7 +13684,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -13798,10 +13798,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -13839,7 +13839,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -14017,16 +14017,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -14372,19 +14372,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -14524,7 +14524,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -14533,7 +14533,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -14647,10 +14647,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -14688,7 +14688,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -14866,16 +14866,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -14993,19 +14993,19 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>23</v>
       </c>
       <c r="E3">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F3">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>76</v>
@@ -15040,10 +15040,10 @@
         <v>17</v>
       </c>
       <c r="E4">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <v>76</v>
@@ -15078,10 +15078,10 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F5">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G5">
         <v>76</v>
@@ -15116,10 +15116,10 @@
         <v>11</v>
       </c>
       <c r="E6">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F6">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G6">
         <v>76</v>
@@ -15154,10 +15154,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G7">
         <v>76</v>
@@ -15183,19 +15183,19 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G8">
         <v>76</v>
@@ -15221,10 +15221,10 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
@@ -15268,10 +15268,10 @@
         <v>16</v>
       </c>
       <c r="E10">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="F10">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="G10">
         <v>76</v>
@@ -15373,7 +15373,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -15382,10 +15382,10 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="G13">
         <v>76</v>
@@ -15420,10 +15420,10 @@
         <v>24</v>
       </c>
       <c r="E14">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F14">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G14">
         <v>76</v>
@@ -15449,19 +15449,19 @@
         <v>25</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15">
         <v>34</v>
       </c>
       <c r="E15">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F15">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G15">
         <v>76</v>
@@ -15496,10 +15496,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F16">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -15534,10 +15534,10 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F17">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -15572,10 +15572,10 @@
         <v>11</v>
       </c>
       <c r="E18">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G18">
         <v>76</v>
@@ -15601,19 +15601,19 @@
         <v>29</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D19">
         <v>36</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G19">
         <v>76</v>
@@ -15686,10 +15686,10 @@
         <v>21</v>
       </c>
       <c r="E21">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="F21">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G21">
         <v>76</v>
@@ -15715,10 +15715,10 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
@@ -15727,7 +15727,7 @@
         <v>41</v>
       </c>
       <c r="F22">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G22">
         <v>76</v>
@@ -16070,19 +16070,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -16222,7 +16222,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -16231,7 +16231,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -16345,10 +16345,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -16386,7 +16386,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -16564,16 +16564,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -16919,19 +16919,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -17071,7 +17071,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -17080,7 +17080,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -17194,10 +17194,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -17235,7 +17235,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -17413,16 +17413,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F22">
         <v>13</v>
@@ -17768,19 +17768,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -17920,7 +17920,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -17929,7 +17929,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -18043,10 +18043,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -18084,7 +18084,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -18262,16 +18262,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -18617,19 +18617,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -18769,7 +18769,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -18778,7 +18778,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -18892,10 +18892,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -18933,7 +18933,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -19111,16 +19111,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -19466,19 +19466,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -19618,7 +19618,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -19627,7 +19627,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -19741,10 +19741,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -19782,7 +19782,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -19960,16 +19960,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -20315,19 +20315,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -20467,7 +20467,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -20476,7 +20476,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -20590,10 +20590,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -20631,7 +20631,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -20809,16 +20809,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -21164,19 +21164,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -21240,19 +21240,19 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <v>38</v>
       </c>
       <c r="E11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G11">
         <v>76</v>
@@ -21316,7 +21316,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -21325,7 +21325,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -21392,7 +21392,7 @@
         <v>25</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -21401,7 +21401,7 @@
         <v>34</v>
       </c>
       <c r="E15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F15">
         <v>3</v>
@@ -21439,10 +21439,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -21480,7 +21480,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -21544,19 +21544,19 @@
         <v>29</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>36</v>
       </c>
       <c r="E19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G19">
         <v>76</v>
@@ -21658,16 +21658,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -22013,19 +22013,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -22165,7 +22165,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -22174,7 +22174,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -22288,10 +22288,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -22329,7 +22329,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -22507,16 +22507,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F22">
         <v>13</v>
@@ -23137,7 +23137,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F16">
         <v>10</v>
@@ -23365,7 +23365,7 @@
         <v>20</v>
       </c>
       <c r="E22">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F22">
         <v>12</v>
@@ -23483,19 +23483,19 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>23</v>
       </c>
       <c r="E3">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F3">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>76</v>
@@ -23530,10 +23530,10 @@
         <v>17</v>
       </c>
       <c r="E4">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <v>76</v>
@@ -23568,10 +23568,10 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F5">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G5">
         <v>76</v>
@@ -23606,10 +23606,10 @@
         <v>11</v>
       </c>
       <c r="E6">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F6">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G6">
         <v>76</v>
@@ -23644,10 +23644,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G7">
         <v>76</v>
@@ -23673,19 +23673,19 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G8">
         <v>76</v>
@@ -23711,10 +23711,10 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
@@ -23758,10 +23758,10 @@
         <v>16</v>
       </c>
       <c r="E10">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="F10">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="G10">
         <v>76</v>
@@ -23863,7 +23863,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -23872,10 +23872,10 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="G13">
         <v>76</v>
@@ -23910,10 +23910,10 @@
         <v>24</v>
       </c>
       <c r="E14">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F14">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G14">
         <v>76</v>
@@ -23939,19 +23939,19 @@
         <v>25</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15">
         <v>34</v>
       </c>
       <c r="E15">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F15">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G15">
         <v>76</v>
@@ -23986,10 +23986,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F16">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -24024,10 +24024,10 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F17">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -24062,10 +24062,10 @@
         <v>11</v>
       </c>
       <c r="E18">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G18">
         <v>76</v>
@@ -24091,19 +24091,19 @@
         <v>29</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D19">
         <v>36</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G19">
         <v>76</v>
@@ -24176,10 +24176,10 @@
         <v>21</v>
       </c>
       <c r="E21">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="F21">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G21">
         <v>76</v>
@@ -24205,10 +24205,10 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
@@ -24217,7 +24217,7 @@
         <v>41</v>
       </c>
       <c r="F22">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G22">
         <v>76</v>
@@ -24332,19 +24332,19 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>23</v>
       </c>
       <c r="E3">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F3">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>76</v>
@@ -24379,10 +24379,10 @@
         <v>17</v>
       </c>
       <c r="E4">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <v>76</v>
@@ -24417,10 +24417,10 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F5">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G5">
         <v>76</v>
@@ -24455,10 +24455,10 @@
         <v>11</v>
       </c>
       <c r="E6">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F6">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G6">
         <v>76</v>
@@ -24493,10 +24493,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G7">
         <v>76</v>
@@ -24522,19 +24522,19 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G8">
         <v>76</v>
@@ -24560,10 +24560,10 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
@@ -24607,10 +24607,10 @@
         <v>16</v>
       </c>
       <c r="E10">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="F10">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="G10">
         <v>76</v>
@@ -24712,7 +24712,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -24721,10 +24721,10 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="G13">
         <v>76</v>
@@ -24759,10 +24759,10 @@
         <v>24</v>
       </c>
       <c r="E14">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F14">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G14">
         <v>76</v>
@@ -24788,19 +24788,19 @@
         <v>25</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15">
         <v>34</v>
       </c>
       <c r="E15">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F15">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G15">
         <v>76</v>
@@ -24835,10 +24835,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F16">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -24873,10 +24873,10 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F17">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -24911,10 +24911,10 @@
         <v>11</v>
       </c>
       <c r="E18">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G18">
         <v>76</v>
@@ -24940,19 +24940,19 @@
         <v>29</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D19">
         <v>36</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G19">
         <v>76</v>
@@ -25025,10 +25025,10 @@
         <v>21</v>
       </c>
       <c r="E21">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="F21">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G21">
         <v>76</v>
@@ -25054,10 +25054,10 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
@@ -25066,7 +25066,7 @@
         <v>41</v>
       </c>
       <c r="F22">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G22">
         <v>76</v>
@@ -25409,19 +25409,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -25561,7 +25561,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -25570,7 +25570,7 @@
         <v>23</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -25684,10 +25684,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -25725,7 +25725,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>76</v>
@@ -25903,16 +25903,16 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>14</v>

</xml_diff>